<commit_message>
cplex separado de gurobi
</commit_message>
<xml_diff>
--- a/Comparar Resultados.xlsx
+++ b/Comparar Resultados.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rablo\Documents\GitHub\CMSTP-TW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BCFDF41-8F8B-4238-8BC6-06398BCCF301}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5438F523-3332-4BD6-BAD1-692329F0B777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="787" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="349">
   <si>
     <t>cplex</t>
   </si>
@@ -1517,7 +1517,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1651,6 +1651,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2359,8 +2360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4AF2F71-FF35-401A-BF65-12EFA2B4DCD7}">
   <dimension ref="A1:Y30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="P19" sqref="P19"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3726,7 +3727,7 @@
         <f>'Q = 5'!BS59</f>
         <v>946.74475648390569</v>
       </c>
-      <c r="G15" s="89">
+      <c r="G15" s="90">
         <f t="shared" si="13"/>
         <v>706.95780065911606</v>
       </c>
@@ -3750,7 +3751,7 @@
         <f>'Q = 5'!BU59</f>
         <v>6.7813298463157548E-2</v>
       </c>
-      <c r="M15" s="54">
+      <c r="M15" s="56">
         <f t="shared" si="14"/>
         <v>4.8571363311831803E-2</v>
       </c>
@@ -3774,7 +3775,7 @@
         <f>'Q = 5'!BV59</f>
         <v>9.0448660666827815E-2</v>
       </c>
-      <c r="S15" s="54">
+      <c r="S15" s="56">
         <f t="shared" si="15"/>
         <v>7.4834795266927295E-2</v>
       </c>
@@ -3798,9 +3799,19 @@
         <f>'Q = 5'!BW59</f>
         <v>18.76137887518437</v>
       </c>
-      <c r="Y15" s="57">
+      <c r="Y15" s="59">
         <f t="shared" si="16"/>
         <v>24.008101370502423</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A16" s="105" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A17" s="105" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
@@ -4049,8 +4060,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BW60"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BW3" sqref="BW3:BW58"/>
+    <sheetView topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18816,12 +18827,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="BI1:BM1"/>
-    <mergeCell ref="BN1:BR1"/>
-    <mergeCell ref="BS1:BW1"/>
-    <mergeCell ref="BD1:BH1"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
     <mergeCell ref="AO1:AS1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="AE1:AI1"/>
@@ -18829,6 +18834,12 @@
     <mergeCell ref="M1:U1"/>
     <mergeCell ref="V1:AD1"/>
     <mergeCell ref="H1:L1"/>
+    <mergeCell ref="BI1:BM1"/>
+    <mergeCell ref="BN1:BR1"/>
+    <mergeCell ref="BS1:BW1"/>
+    <mergeCell ref="BD1:BH1"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18838,8 +18849,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEB5D206-0A24-468D-A765-C918D296F42E}">
   <dimension ref="A1:BW60"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BW3" sqref="BW3:BW58"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33659,12 +33670,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="BN1:BR1"/>
-    <mergeCell ref="BS1:BW1"/>
-    <mergeCell ref="BI1:BM1"/>
-    <mergeCell ref="BD1:BH1"/>
-    <mergeCell ref="AT1:AX1"/>
-    <mergeCell ref="AY1:BC1"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="M1:U1"/>
     <mergeCell ref="V1:AD1"/>
@@ -33672,6 +33677,12 @@
     <mergeCell ref="AE1:AI1"/>
     <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="H1:L1"/>
+    <mergeCell ref="BN1:BR1"/>
+    <mergeCell ref="BS1:BW1"/>
+    <mergeCell ref="BI1:BM1"/>
+    <mergeCell ref="BD1:BH1"/>
+    <mergeCell ref="AT1:AX1"/>
+    <mergeCell ref="AY1:BC1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>